<commit_message>
Verify hotel searc critria
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/data - Copy.xlsx
+++ b/src/test/resources/testData/data - Copy.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BWI_Assignment\bestwestern\src\test\resources\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Wk\bwiRepo\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -38,9 +38,6 @@
     <t>CheckOutMonth</t>
   </si>
   <si>
-    <t>New York, NY, USA</t>
-  </si>
-  <si>
     <t xml:space="preserve">CheckInMonth </t>
   </si>
   <si>
@@ -48,6 +45,9 @@
   </si>
   <si>
     <t>Canberra ACT, Australia</t>
+  </si>
+  <si>
+    <t>Chicago, IL, USA</t>
   </si>
 </sst>
 </file>
@@ -391,7 +391,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,7 +407,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -421,16 +421,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2">
         <v>24</v>
@@ -438,16 +438,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3">
         <v>27</v>

</xml_diff>